<commit_message>
Updated Mouser order list and added comment to README
</commit_message>
<xml_diff>
--- a/hardware/pcb/Mouser Parts Order.xlsx
+++ b/hardware/pcb/Mouser Parts Order.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\Projects\FolkraceCar\hardware\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A484F869-67D2-4981-B8FC-0772E35054B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B70AEFB-8746-4E32-ADEB-97418837562B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="7125" windowWidth="12150" windowHeight="14475"/>
+    <workbookView xWindow="38280" yWindow="-4065" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,12 +19,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'kicad csv import'!$F$1:$F$31</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="153">
   <si>
     <t>Reference</t>
   </si>
@@ -420,12 +428,75 @@
   </si>
   <si>
     <t>Copy paste</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Recieved</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>ADS1015BQDGSRQ1</t>
+  </si>
+  <si>
+    <t>595-ADS1015BQDGSRQ1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>Raspberry_Pi Header</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Adafruit: 2222</t>
+  </si>
+  <si>
+    <t>485-2222</t>
+  </si>
+  <si>
+    <t>SW2 SW3</t>
+  </si>
+  <si>
+    <t>B3U-1000P-B</t>
+  </si>
+  <si>
+    <t>Omron Electronics</t>
+  </si>
+  <si>
+    <t>653-B3U-1000P-B</t>
+  </si>
+  <si>
+    <t>M2.5 standoff 11 mm</t>
+  </si>
+  <si>
+    <t>710-970110151</t>
+  </si>
+  <si>
+    <t>Wurth Elektronik</t>
+  </si>
+  <si>
+    <t>M2.5 standoff 5+6 mm</t>
+  </si>
+  <si>
+    <t>710-971050154</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>534-29300</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1259,349 +1330,530 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>129</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="str">
+        <f>H2&amp;","&amp;"Folkrace laZEr"&amp;","&amp;E2</f>
+        <v>963-TMK105B7104MV-FR,Folkrace laZEr,10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J16" si="0">H3&amp;","&amp;"Folkrace laZEr"&amp;","&amp;E3</f>
+        <v>963-TMK316AB7106KL-T,Folkrace laZEr,10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>963-TMF105B7223KVHF,Folkrace laZEr,10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>595-DRV8874PWPR,Folkrace laZEr,1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>538-39-30-0020,Folkrace laZEr,4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>660-TLRZ1JTTD,Folkrace laZEr,2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>863-MGSF2N02ELT1G,Folkrace laZEr,2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>100</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="str">
-        <f>G2&amp;","&amp;"Folkrace laZEr"&amp;","&amp;D2</f>
-        <v>963-TMK105B7104MV-FR,Folkrace laZEr,100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>653-A6S-1102-PH,Folkrace laZEr,1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I11" si="0">G3&amp;","&amp;"Folkrace laZEr"&amp;","&amp;D3</f>
-        <v>963-TMK316AB7106KL-T,Folkrace laZEr,10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>595-TPS25940LQRVCRQ1,Folkrace laZEr,2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>963-TMF105B7223KVHF,Folkrace laZEr,100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
+        <v>595-ADS1015BQDGSRQ1,Folkrace laZEr,1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>485-2222,Folkrace laZEr,1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" t="s">
+        <v>145</v>
+      </c>
+      <c r="I13" t="s">
         <v>19</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J13" t="str">
         <f t="shared" si="0"/>
-        <v>595-DRV8874PWPR,Folkrace laZEr,2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" t="s">
+        <v>653-B3U-1000P-B,Folkrace laZEr,2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14">
+        <v>970110151</v>
+      </c>
+      <c r="H14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" t="s">
         <v>19</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J14" t="str">
         <f t="shared" si="0"/>
-        <v>538-39-30-0020,Folkrace laZEr,5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" t="s">
+        <v>710-970110151,Folkrace laZEr,4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15">
+        <v>971050154</v>
+      </c>
+      <c r="H15" t="s">
+        <v>150</v>
+      </c>
+      <c r="I15" t="s">
         <v>19</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J15" t="str">
         <f t="shared" si="0"/>
-        <v>660-TLRZ1JTTD,Folkrace laZEr,5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8" t="s">
+        <v>710-971050154,Folkrace laZEr,4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16">
+        <v>29300</v>
+      </c>
+      <c r="H16" t="s">
+        <v>152</v>
+      </c>
+      <c r="I16" t="s">
         <v>19</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J16" t="str">
         <f t="shared" si="0"/>
-        <v>863-MGSF2N02ELT1G,Folkrace laZEr,10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" t="s">
+        <v>534-29300,Folkrace laZEr,4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>124</v>
+      </c>
+      <c r="H28" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" t="s">
         <v>19</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>653-A6S-1102-PH,Folkrace laZEr,2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>595-TPS25940LQRVCRQ1,Folkrace laZEr,3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>124</v>
-      </c>
-      <c r="G11" t="s">
-        <v>127</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
+      <c r="J28" t="str">
+        <f>H28&amp;","&amp;"Folkrace laZEr"&amp;","&amp;E28</f>
         <v>580-OKL-T/6-W12N-C,Folkrace laZEr,0</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{26A76689-DEA1-424B-BC67-52C7531C1AAF}">
+      <formula1>"Ordered, Recieved"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K31"/>
   <sheetViews>
@@ -2291,7 +2543,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F31">
+  <autoFilter ref="F1:F31" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>

</xml_diff>